<commit_message>
Fixing column names in column-name-sheet
</commit_message>
<xml_diff>
--- a/Tools/columns.xlsx
+++ b/Tools/columns.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\GIT\fetlife-aslsearch-reborn\Tools\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F36BCC9-6478-42E2-A44D-160BAB3F1EAD}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF85B825-AD74-42F0-84BC-11E2F37CD1A3}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2240" yWindow="2240" windowWidth="28800" windowHeight="15460" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2240" yWindow="2240" windowWidth="35930" windowHeight="15460" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,81 +20,93 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
-  <si>
-    <t>Gender</t>
-  </si>
-  <si>
-    <t>Role</t>
-  </si>
-  <si>
-    <t>Friend Count</t>
-  </si>
-  <si>
-    <t>Paid Account?</t>
-  </si>
-  <si>
-    <t>Locality</t>
-  </si>
-  <si>
-    <t>Region</t>
-  </si>
-  <si>
-    <t>Country</t>
-  </si>
-  <si>
-    <t>Avatar URL</t>
-  </si>
-  <si>
-    <t>Sexual Orientation</t>
-  </si>
-  <si>
-    <t>Interest Level ("Active")</t>
-  </si>
-  <si>
-    <t>Looking For</t>
-  </si>
-  <si>
-    <t>Vanilla Relationships</t>
-  </si>
-  <si>
-    <t>D/s Relationships</t>
-  </si>
-  <si>
-    <t>Bio ("About Me")</t>
-  </si>
-  <si>
-    <t>Websites</t>
-  </si>
-  <si>
-    <t>Last Activity</t>
-  </si>
-  <si>
-    <t>Fetishes Into</t>
-  </si>
-  <si>
-    <t>Fetishes Curious About</t>
-  </si>
-  <si>
-    <t>Number of Pictures</t>
-  </si>
-  <si>
-    <t>Number of Videos</t>
-  </si>
-  <si>
-    <t>Latest Writings</t>
-  </si>
-  <si>
-    <t>Groups Lead</t>
-  </si>
-  <si>
-    <t>Groups Member Of</t>
-  </si>
-  <si>
-    <t>Events Going To</t>
-  </si>
-  <si>
-    <t>Events Maybe Going To</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="29">
+  <si>
+    <t>last_updated</t>
+  </si>
+  <si>
+    <t>age</t>
+  </si>
+  <si>
+    <t>nickname</t>
+  </si>
+  <si>
+    <t>user_id</t>
+  </si>
+  <si>
+    <t>gender</t>
+  </si>
+  <si>
+    <t>friend_count</t>
+  </si>
+  <si>
+    <t>paid_account</t>
+  </si>
+  <si>
+    <t>fetishes_curious_about</t>
+  </si>
+  <si>
+    <t>events_maybe_going_to</t>
+  </si>
+  <si>
+    <t>events_going_to</t>
+  </si>
+  <si>
+    <t>groups_member_of</t>
+  </si>
+  <si>
+    <t>groups_lead</t>
+  </si>
+  <si>
+    <t>latest_posts</t>
+  </si>
+  <si>
+    <t>num_vids</t>
+  </si>
+  <si>
+    <t>num_pics</t>
+  </si>
+  <si>
+    <t>fetishes_into</t>
+  </si>
+  <si>
+    <t>last_activity</t>
+  </si>
+  <si>
+    <t>websites</t>
+  </si>
+  <si>
+    <t>bio</t>
+  </si>
+  <si>
+    <t>ds_relationships</t>
+  </si>
+  <si>
+    <t>relationships</t>
+  </si>
+  <si>
+    <t>looking_for</t>
+  </si>
+  <si>
+    <t>interest_level</t>
+  </si>
+  <si>
+    <t>sexual_orientation</t>
+  </si>
+  <si>
+    <t>avatar_url</t>
+  </si>
+  <si>
+    <t>location_country</t>
+  </si>
+  <si>
+    <t>location_region</t>
+  </si>
+  <si>
+    <t>location_locality</t>
+  </si>
+  <si>
+    <t>role</t>
   </si>
 </sst>
 </file>
@@ -130,8 +142,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standaard" xfId="0" builtinId="0"/>
@@ -473,101 +488,102 @@
   <dimension ref="A1:AC1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
     <row r="1" spans="1:29" x14ac:dyDescent="0.35">
-      <c r="A1">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B1">
-        <v>2</v>
-      </c>
-      <c r="C1">
-        <v>3</v>
-      </c>
-      <c r="D1">
+      <c r="E1" t="s">
         <v>4</v>
       </c>
-      <c r="E1" t="s">
-        <v>0</v>
-      </c>
       <c r="F1" t="s">
-        <v>1</v>
+        <v>28</v>
       </c>
       <c r="G1" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="H1" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="I1" t="s">
-        <v>4</v>
+        <v>27</v>
       </c>
       <c r="J1" t="s">
-        <v>5</v>
+        <v>26</v>
       </c>
       <c r="K1" t="s">
-        <v>6</v>
+        <v>25</v>
       </c>
       <c r="L1" t="s">
+        <v>24</v>
+      </c>
+      <c r="M1" t="s">
+        <v>23</v>
+      </c>
+      <c r="N1" t="s">
+        <v>22</v>
+      </c>
+      <c r="O1" t="s">
+        <v>21</v>
+      </c>
+      <c r="P1" t="s">
+        <v>20</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>19</v>
+      </c>
+      <c r="R1" t="s">
+        <v>18</v>
+      </c>
+      <c r="S1" t="s">
+        <v>17</v>
+      </c>
+      <c r="T1" t="s">
+        <v>16</v>
+      </c>
+      <c r="U1" t="s">
+        <v>15</v>
+      </c>
+      <c r="V1" t="s">
         <v>7</v>
       </c>
-      <c r="M1" t="s">
+      <c r="W1" t="s">
+        <v>14</v>
+      </c>
+      <c r="X1" t="s">
+        <v>13</v>
+      </c>
+      <c r="Y1" t="s">
+        <v>12</v>
+      </c>
+      <c r="Z1" t="s">
+        <v>11</v>
+      </c>
+      <c r="AA1" t="s">
+        <v>10</v>
+      </c>
+      <c r="AB1" t="s">
+        <v>9</v>
+      </c>
+      <c r="AC1" t="s">
         <v>8</v>
-      </c>
-      <c r="N1" t="s">
-        <v>9</v>
-      </c>
-      <c r="O1" t="s">
-        <v>10</v>
-      </c>
-      <c r="P1" t="s">
-        <v>11</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>12</v>
-      </c>
-      <c r="R1" t="s">
-        <v>13</v>
-      </c>
-      <c r="S1" t="s">
-        <v>14</v>
-      </c>
-      <c r="T1" t="s">
-        <v>15</v>
-      </c>
-      <c r="U1" t="s">
-        <v>16</v>
-      </c>
-      <c r="V1" t="s">
-        <v>17</v>
-      </c>
-      <c r="W1" t="s">
-        <v>18</v>
-      </c>
-      <c r="X1" t="s">
-        <v>19</v>
-      </c>
-      <c r="Y1" t="s">
-        <v>20</v>
-      </c>
-      <c r="Z1" t="s">
-        <v>21</v>
-      </c>
-      <c r="AA1" t="s">
-        <v>22</v>
-      </c>
-      <c r="AB1" t="s">
-        <v>23</v>
-      </c>
-      <c r="AC1" t="s">
-        <v>24</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>